<commit_message>
Playing aroudn with the SH data
</commit_message>
<xml_diff>
--- a/Nitrogen Isotope Data.xlsx
+++ b/Nitrogen Isotope Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashitt/Dropbox/Marsden Black Coral Project/R Codes/Hitt-et-al-2022-Bulk-N-Isotopes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6EBDD7-E159-7045-B1E7-290C842919B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814BDBA1-97DA-8944-BB01-D02C39D4E00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5860" yWindow="1460" windowWidth="27240" windowHeight="15740" xr2:uid="{478DFB51-A313-FF43-AAC3-7EF788E91FA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="6">
   <si>
     <t>err</t>
   </si>
@@ -47,12 +47,18 @@
   <si>
     <t>age</t>
   </si>
+  <si>
+    <t>SH9</t>
+  </si>
+  <si>
+    <t>SH10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,6 +77,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -220,6 +232,2493 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$378:$A$439</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>594</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>616</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>638</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>659</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>681</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>703</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>811</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>855</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>876</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>898</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>941</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>963</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1032</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1067</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1136</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1205</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1252</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1346</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1393</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1487</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1527</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1540</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1553</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1592</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1606</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1619</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1645</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1671</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1685</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1698</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1711</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1832</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1872</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1913</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2114</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2155</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2195</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2235</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2275</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2316</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2356</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2396</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$378:$B$439</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="62"/>
+                <c:pt idx="0">
+                  <c:v>12.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.88</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.99</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.02</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.96</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.95</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.46</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.79</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.97</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.79</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.06</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11.94</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12.11</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.03</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12.12</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12.04</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11.95</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11.78</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11.96</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12.08</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11.93</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11.97</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11.72</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11.83</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11.91</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11.93</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11.94</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12.01</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12.22</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>11.97</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12.03</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>12.24</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>11.72</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>11.87</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>12.06</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>11.71</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>11.72</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>12.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DC1-334F-A0E7-9F92D0420B35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="149612863"/>
+        <c:axId val="7534015"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="149612863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7534015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="7534015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="149612863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$439:$A$496</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2530.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2561.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2592.77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2623.69</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2654.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2685.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2716.46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2747.38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2778.31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2809.23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2840.15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2871.08</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2902</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2932.92</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2994.77</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3025.69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3056.62</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3118.46</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3180.31</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3211.23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3242.15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3273.08</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3304</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3334.92</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3365.85</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3396.77</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3427.69</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3458.62</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3489.54</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3520.46</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3551.38</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3582.31</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3644.15</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3675.08</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3706</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3736.92</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3767.85</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3798.77</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3829.69</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3860.62</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3922.46</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3953.38</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3984.31</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4046.15</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4077.08</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4108</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4169.8500000000004</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4200.7700000000004</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4231.6899999999996</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4262.62</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4293.54</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4324.46</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4355.38</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4417.2299999999996</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4448.1499999999996</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4479.08</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4510</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$439:$B$496</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>12.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.86</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.98</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.04</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.82</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.74</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.83</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.09002128</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.088571119999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12.13789674</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.861946400000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.66517423</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.90426622</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.78796277</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.94842176</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.87841405</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.59</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.67</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.77</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11.65</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.89</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.98</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12.22</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12.16464081</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.006327649999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11.950292490000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.05391861</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>11.69609337</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11.78448206</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12.06</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11.79</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11.63</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11.96</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11.98</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12.16</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12.53</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12.37</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>12.34</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12.33</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>12.28</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6041-9842-9E7D-C58C4D59E6A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="7456159"/>
+        <c:axId val="169407679"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="7456159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="169407679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="169407679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7456159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>372</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>391</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EED785FC-92C6-8042-872D-2965A77EAC6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>473</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>492</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2F18D0C-174B-434D-A3E8-F4C7C7E74886}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,10 +3018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D8330C-6A64-4F4C-B23C-81ECA811C9CC}">
-  <dimension ref="A1:D377"/>
+  <dimension ref="A1:D496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112:B181"/>
+    <sheetView tabSelected="1" topLeftCell="A468" workbookViewId="0">
+      <selection activeCell="A493" sqref="A493:XFD493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5805,7 +8304,1318 @@
         <v>35104</v>
       </c>
     </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A378">
+        <v>491</v>
+      </c>
+      <c r="B378">
+        <v>12.07</v>
+      </c>
+      <c r="D378" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A379">
+        <v>511</v>
+      </c>
+      <c r="B379">
+        <v>12.03</v>
+      </c>
+      <c r="D379" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <v>531</v>
+      </c>
+      <c r="B380">
+        <v>12.41</v>
+      </c>
+      <c r="D380" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A381">
+        <v>551</v>
+      </c>
+      <c r="B381">
+        <v>12.57</v>
+      </c>
+      <c r="D381" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A382">
+        <v>573</v>
+      </c>
+      <c r="B382">
+        <v>12.27</v>
+      </c>
+      <c r="D382" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A383">
+        <v>594</v>
+      </c>
+      <c r="B383">
+        <v>12.34</v>
+      </c>
+      <c r="D383" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A384">
+        <v>616</v>
+      </c>
+      <c r="B384">
+        <v>12.47</v>
+      </c>
+      <c r="D384" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A385">
+        <v>638</v>
+      </c>
+      <c r="B385">
+        <v>12.7</v>
+      </c>
+      <c r="D385" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A386">
+        <v>659</v>
+      </c>
+      <c r="B386">
+        <v>12.45</v>
+      </c>
+      <c r="D386" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A387">
+        <v>681</v>
+      </c>
+      <c r="B387">
+        <v>12.54</v>
+      </c>
+      <c r="D387" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A388">
+        <v>703</v>
+      </c>
+      <c r="B388">
+        <v>12.08</v>
+      </c>
+      <c r="D388" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A389">
+        <v>724</v>
+      </c>
+      <c r="B389">
+        <v>12.35</v>
+      </c>
+      <c r="D389" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A390">
+        <v>746</v>
+      </c>
+      <c r="B390">
+        <v>12.15</v>
+      </c>
+      <c r="D390" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A391">
+        <v>768</v>
+      </c>
+      <c r="B391">
+        <v>11.65</v>
+      </c>
+      <c r="D391" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A392">
+        <v>790</v>
+      </c>
+      <c r="B392">
+        <v>11.88</v>
+      </c>
+      <c r="D392" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A393">
+        <v>811</v>
+      </c>
+      <c r="B393">
+        <v>12.14</v>
+      </c>
+      <c r="D393" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <v>833</v>
+      </c>
+      <c r="B394">
+        <v>12.19</v>
+      </c>
+      <c r="D394" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <v>855</v>
+      </c>
+      <c r="B395">
+        <v>12.27</v>
+      </c>
+      <c r="D395" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <v>876</v>
+      </c>
+      <c r="B396">
+        <v>11.99</v>
+      </c>
+      <c r="D396" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A397">
+        <v>898</v>
+      </c>
+      <c r="B397">
+        <v>12.02</v>
+      </c>
+      <c r="D397" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A398">
+        <v>920</v>
+      </c>
+      <c r="B398">
+        <v>12</v>
+      </c>
+      <c r="D398" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A399">
+        <v>941</v>
+      </c>
+      <c r="B399">
+        <v>11.96</v>
+      </c>
+      <c r="D399" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A400">
+        <v>963</v>
+      </c>
+      <c r="B400">
+        <v>11.95</v>
+      </c>
+      <c r="D400" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A401">
+        <v>998</v>
+      </c>
+      <c r="B401">
+        <v>11.46</v>
+      </c>
+      <c r="D401" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <v>1032</v>
+      </c>
+      <c r="B402">
+        <v>11.62</v>
+      </c>
+      <c r="D402" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>1067</v>
+      </c>
+      <c r="B403">
+        <v>11.79</v>
+      </c>
+      <c r="D403" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>1136</v>
+      </c>
+      <c r="B404">
+        <v>11.97</v>
+      </c>
+      <c r="D404" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>1205</v>
+      </c>
+      <c r="B405">
+        <v>11.79</v>
+      </c>
+      <c r="D405" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>1252</v>
+      </c>
+      <c r="B406">
+        <v>12.06</v>
+      </c>
+      <c r="D406" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>1346</v>
+      </c>
+      <c r="B407">
+        <v>12.3</v>
+      </c>
+      <c r="D407" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>1393</v>
+      </c>
+      <c r="B408">
+        <v>11.94</v>
+      </c>
+      <c r="D408" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <v>1440</v>
+      </c>
+      <c r="B409">
+        <v>11.5</v>
+      </c>
+      <c r="D409" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <v>1487</v>
+      </c>
+      <c r="B410">
+        <v>12.11</v>
+      </c>
+      <c r="D410" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <v>1500</v>
+      </c>
+      <c r="B411">
+        <v>12.03</v>
+      </c>
+      <c r="D411" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <v>1527</v>
+      </c>
+      <c r="B412">
+        <v>12.12</v>
+      </c>
+      <c r="D412" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <v>1540</v>
+      </c>
+      <c r="B413">
+        <v>12.04</v>
+      </c>
+      <c r="D413" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <v>1553</v>
+      </c>
+      <c r="B414">
+        <v>11.95</v>
+      </c>
+      <c r="D414" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <v>1592</v>
+      </c>
+      <c r="B415">
+        <v>11.7</v>
+      </c>
+      <c r="D415" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <v>1606</v>
+      </c>
+      <c r="B416">
+        <v>11.78</v>
+      </c>
+      <c r="D416" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>1619</v>
+      </c>
+      <c r="B417">
+        <v>11.96</v>
+      </c>
+      <c r="D417" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <v>1632</v>
+      </c>
+      <c r="B418">
+        <v>12.08</v>
+      </c>
+      <c r="D418" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <v>1645</v>
+      </c>
+      <c r="B419">
+        <v>11.93</v>
+      </c>
+      <c r="D419" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>1671</v>
+      </c>
+      <c r="B420">
+        <v>12</v>
+      </c>
+      <c r="D420" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>1685</v>
+      </c>
+      <c r="B421">
+        <v>11.97</v>
+      </c>
+      <c r="D421" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>1698</v>
+      </c>
+      <c r="B422">
+        <v>11.72</v>
+      </c>
+      <c r="D422" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>1711</v>
+      </c>
+      <c r="B423">
+        <v>11.83</v>
+      </c>
+      <c r="D423" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>1792</v>
+      </c>
+      <c r="B424">
+        <v>11.91</v>
+      </c>
+      <c r="D424" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>1832</v>
+      </c>
+      <c r="B425">
+        <v>11.93</v>
+      </c>
+      <c r="D425" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>1872</v>
+      </c>
+      <c r="B426">
+        <v>11.94</v>
+      </c>
+      <c r="D426" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <v>1913</v>
+      </c>
+      <c r="B427">
+        <v>12.01</v>
+      </c>
+      <c r="D427" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>1953</v>
+      </c>
+      <c r="B428">
+        <v>12.25</v>
+      </c>
+      <c r="D428" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>1993</v>
+      </c>
+      <c r="B429">
+        <v>12.22</v>
+      </c>
+      <c r="D429" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>2034</v>
+      </c>
+      <c r="B430">
+        <v>11.97</v>
+      </c>
+      <c r="D430" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>2114</v>
+      </c>
+      <c r="B431">
+        <v>12.03</v>
+      </c>
+      <c r="D431" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>2155</v>
+      </c>
+      <c r="B432">
+        <v>12.24</v>
+      </c>
+      <c r="D432" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>2195</v>
+      </c>
+      <c r="B433">
+        <v>11.72</v>
+      </c>
+      <c r="D433" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>2235</v>
+      </c>
+      <c r="B434">
+        <v>11.87</v>
+      </c>
+      <c r="D434" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>2275</v>
+      </c>
+      <c r="B435">
+        <v>12.06</v>
+      </c>
+      <c r="D435" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <v>2316</v>
+      </c>
+      <c r="B436">
+        <v>11.71</v>
+      </c>
+      <c r="D436" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <v>2356</v>
+      </c>
+      <c r="B437">
+        <v>11.8</v>
+      </c>
+      <c r="D437" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>2396</v>
+      </c>
+      <c r="B438">
+        <v>11.72</v>
+      </c>
+      <c r="D438" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>2500</v>
+      </c>
+      <c r="B439">
+        <v>12.09</v>
+      </c>
+      <c r="D439" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>2530.92</v>
+      </c>
+      <c r="B440">
+        <v>11.98</v>
+      </c>
+      <c r="D440" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>2561.85</v>
+      </c>
+      <c r="B441">
+        <v>11.88</v>
+      </c>
+      <c r="D441" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <v>2592.77</v>
+      </c>
+      <c r="B442">
+        <v>11.77</v>
+      </c>
+      <c r="D442" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <v>2623.69</v>
+      </c>
+      <c r="B443">
+        <v>11.73</v>
+      </c>
+      <c r="D443" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <v>2654.62</v>
+      </c>
+      <c r="B444">
+        <v>11.92</v>
+      </c>
+      <c r="D444" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <v>2685.54</v>
+      </c>
+      <c r="B445">
+        <v>12.02</v>
+      </c>
+      <c r="D445" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <v>2716.46</v>
+      </c>
+      <c r="B446">
+        <v>11.86</v>
+      </c>
+      <c r="D446" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <v>2747.38</v>
+      </c>
+      <c r="B447">
+        <v>12.05</v>
+      </c>
+      <c r="D447" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <v>2778.31</v>
+      </c>
+      <c r="B448">
+        <v>11.98</v>
+      </c>
+      <c r="D448" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A449">
+        <v>2809.23</v>
+      </c>
+      <c r="B449">
+        <v>12.33</v>
+      </c>
+      <c r="D449" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A450">
+        <v>2840.15</v>
+      </c>
+      <c r="B450">
+        <v>12.25</v>
+      </c>
+      <c r="D450" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A451">
+        <v>2871.08</v>
+      </c>
+      <c r="B451">
+        <v>12.04</v>
+      </c>
+      <c r="D451" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A452">
+        <v>2902</v>
+      </c>
+      <c r="B452">
+        <v>12.01</v>
+      </c>
+      <c r="D452" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A453">
+        <v>2932.92</v>
+      </c>
+      <c r="B453">
+        <v>12.11</v>
+      </c>
+      <c r="D453" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A454">
+        <v>2994.77</v>
+      </c>
+      <c r="B454">
+        <v>11.82</v>
+      </c>
+      <c r="D454" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A455">
+        <v>3025.69</v>
+      </c>
+      <c r="B455">
+        <v>11.74</v>
+      </c>
+      <c r="D455" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A456">
+        <v>3056.62</v>
+      </c>
+      <c r="B456">
+        <v>11.83</v>
+      </c>
+      <c r="D456" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A457">
+        <v>3118.46</v>
+      </c>
+      <c r="B457">
+        <v>12.09002128</v>
+      </c>
+      <c r="D457" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A458">
+        <v>3180.31</v>
+      </c>
+      <c r="B458">
+        <v>12.088571119999999</v>
+      </c>
+      <c r="D458" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A459">
+        <v>3211.23</v>
+      </c>
+      <c r="B459">
+        <v>12.13789674</v>
+      </c>
+      <c r="D459" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A460">
+        <v>3242.15</v>
+      </c>
+      <c r="B460">
+        <v>11.861946400000001</v>
+      </c>
+      <c r="D460" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A461">
+        <v>3273.08</v>
+      </c>
+      <c r="B461">
+        <v>11.66517423</v>
+      </c>
+      <c r="D461" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <v>3304</v>
+      </c>
+      <c r="B462">
+        <v>11.90426622</v>
+      </c>
+      <c r="D462" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <v>3334.92</v>
+      </c>
+      <c r="B463">
+        <v>11.78796277</v>
+      </c>
+      <c r="D463" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <v>3365.85</v>
+      </c>
+      <c r="B464">
+        <v>11.94842176</v>
+      </c>
+      <c r="D464" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A465">
+        <v>3396.77</v>
+      </c>
+      <c r="B465">
+        <v>11.87841405</v>
+      </c>
+      <c r="D465" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A466">
+        <v>3427.69</v>
+      </c>
+      <c r="B466">
+        <v>11.59</v>
+      </c>
+      <c r="D466" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <v>3458.62</v>
+      </c>
+      <c r="B467">
+        <v>11.67</v>
+      </c>
+      <c r="D467" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <v>3489.54</v>
+      </c>
+      <c r="B468">
+        <v>11.77</v>
+      </c>
+      <c r="D468" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A469">
+        <v>3520.46</v>
+      </c>
+      <c r="B469">
+        <v>11.65</v>
+      </c>
+      <c r="D469" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A470">
+        <v>3551.38</v>
+      </c>
+      <c r="B470">
+        <v>11.89</v>
+      </c>
+      <c r="D470" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A471">
+        <v>3582.31</v>
+      </c>
+      <c r="B471">
+        <v>12.25</v>
+      </c>
+      <c r="D471" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A472">
+        <v>3644.15</v>
+      </c>
+      <c r="B472">
+        <v>12.2</v>
+      </c>
+      <c r="D472" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A473">
+        <v>3675.08</v>
+      </c>
+      <c r="B473">
+        <v>11.98</v>
+      </c>
+      <c r="D473" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A474">
+        <v>3706</v>
+      </c>
+      <c r="B474">
+        <v>12.22</v>
+      </c>
+      <c r="D474" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A475">
+        <v>3736.92</v>
+      </c>
+      <c r="B475">
+        <v>12.16464081</v>
+      </c>
+      <c r="D475" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A476">
+        <v>3767.85</v>
+      </c>
+      <c r="B476">
+        <v>12.006327649999999</v>
+      </c>
+      <c r="D476" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A477">
+        <v>3798.77</v>
+      </c>
+      <c r="B477">
+        <v>11.950292490000001</v>
+      </c>
+      <c r="D477" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A478">
+        <v>3829.69</v>
+      </c>
+      <c r="B478">
+        <v>12.05391861</v>
+      </c>
+      <c r="D478" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A479">
+        <v>3860.62</v>
+      </c>
+      <c r="B479">
+        <v>11.69609337</v>
+      </c>
+      <c r="D479" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A480">
+        <v>3922.46</v>
+      </c>
+      <c r="B480">
+        <v>11.78448206</v>
+      </c>
+      <c r="D480" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A481">
+        <v>3953.38</v>
+      </c>
+      <c r="B481">
+        <v>12.06</v>
+      </c>
+      <c r="D481" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A482">
+        <v>3984.31</v>
+      </c>
+      <c r="B482">
+        <v>11.79</v>
+      </c>
+      <c r="D482" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A483">
+        <v>4046.15</v>
+      </c>
+      <c r="B483">
+        <v>11.9</v>
+      </c>
+      <c r="D483" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A484">
+        <v>4077.08</v>
+      </c>
+      <c r="B484">
+        <v>11.63</v>
+      </c>
+      <c r="D484" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A485">
+        <v>4108</v>
+      </c>
+      <c r="B485">
+        <v>11.96</v>
+      </c>
+      <c r="D485" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A486">
+        <v>4169.8500000000004</v>
+      </c>
+      <c r="B486">
+        <v>11.98</v>
+      </c>
+      <c r="D486" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A487">
+        <v>4200.7700000000004</v>
+      </c>
+      <c r="B487">
+        <v>12.16</v>
+      </c>
+      <c r="D487" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A488">
+        <v>4231.6899999999996</v>
+      </c>
+      <c r="B488">
+        <v>12.1</v>
+      </c>
+      <c r="D488" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A489">
+        <v>4262.62</v>
+      </c>
+      <c r="B489">
+        <v>12.53</v>
+      </c>
+      <c r="D489" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A490">
+        <v>4293.54</v>
+      </c>
+      <c r="B490">
+        <v>12.37</v>
+      </c>
+      <c r="D490" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A491">
+        <v>4324.46</v>
+      </c>
+      <c r="B491">
+        <v>12.34</v>
+      </c>
+      <c r="D491" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A492">
+        <v>4355.38</v>
+      </c>
+      <c r="B492">
+        <v>12.33</v>
+      </c>
+      <c r="D492" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A493">
+        <v>4417.2299999999996</v>
+      </c>
+      <c r="B493">
+        <v>12.3</v>
+      </c>
+      <c r="D493" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A494">
+        <v>4448.1499999999996</v>
+      </c>
+      <c r="B494">
+        <v>12.28</v>
+      </c>
+      <c r="D494" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A495">
+        <v>4479.08</v>
+      </c>
+      <c r="B495">
+        <v>12.25</v>
+      </c>
+      <c r="D495" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A496">
+        <v>4510</v>
+      </c>
+      <c r="B496">
+        <v>11.92</v>
+      </c>
+      <c r="D496" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>